<commit_message>
committing changes for few scripts
</commit_message>
<xml_diff>
--- a/Mendix/input/Mendix_TestPlan.xlsx
+++ b/Mendix/input/Mendix_TestPlan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="336">
   <si>
     <t>S.NO</t>
   </si>
@@ -1017,6 +1017,18 @@
   </si>
   <si>
     <t>Create with ref Global Only - SAP Direct Copy with Rejections</t>
+  </si>
+  <si>
+    <t>Create Vendor Happy flow - with disable Local and Bank Request(SAP)</t>
+  </si>
+  <si>
+    <t>1420073</t>
+  </si>
+  <si>
+    <t>503159</t>
+  </si>
+  <si>
+    <t>Create Material with Questionnaire only Global - SAP Duplicate Found, Extend Selected</t>
   </si>
 </sst>
 </file>
@@ -1417,10 +1429,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:IV10"/>
+  <dimension ref="A1:IV12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2621,7 +2633,7 @@
         <v>331</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>257</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>329</v>
@@ -2643,6 +2655,76 @@
       </c>
       <c r="K10" s="2">
         <v>34413</v>
+      </c>
+    </row>
+    <row r="11" spans="1:255" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:255" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing More missing methods
</commit_message>
<xml_diff>
--- a/Mendix/input/Mendix_TestPlan.xlsx
+++ b/Mendix/input/Mendix_TestPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Git\MIP\Mendix\input\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="340">
   <si>
     <t>S.NO</t>
   </si>
@@ -1029,12 +1029,25 @@
   </si>
   <si>
     <t>Create Material with Questionnaire only Global - SAP Duplicate Found, Extend Selected</t>
+  </si>
+  <si>
+    <t>Create_Vendor_with_Questionnaire_with_Global_and_Local_JDE</t>
+  </si>
+  <si>
+    <t>SG04</t>
+  </si>
+  <si>
+    <t>1332996</t>
+  </si>
+  <si>
+    <t>14835</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1076,7 +1089,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1089,6 +1102,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1429,30 +1445,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:IV12"/>
+  <dimension ref="A1:IV13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="75.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="14.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="256" width="9.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="9.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="75.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="11.109375" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" style="1" width="14.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="12.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="12.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="10.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="23.109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="23.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="12.44140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="12.33203125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="1" width="12.44140625" collapsed="true"/>
+    <col min="17" max="256" customWidth="true" style="1" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2703,7 +2719,7 @@
         <v>335</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>24</v>
+        <v>257</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>333</v>
@@ -2725,6 +2741,41 @@
       </c>
       <c r="K12" s="2" t="s">
         <v>334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:255" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -2748,14 +2799,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="55" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="55" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="254" width="9.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="255" max="255" width="4.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="256" max="256" width="55" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="4.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="55.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="24.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="28.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="55.0" collapsed="true"/>
+    <col min="6" max="254" customWidth="true" style="1" width="9.109375" collapsed="true"/>
+    <col min="255" max="255" customWidth="true" style="1" width="4.88671875" collapsed="true"/>
+    <col min="256" max="256" customWidth="true" style="1" width="55.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2881,9 +2932,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="123.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="256" width="9.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="22.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="123.109375" collapsed="true"/>
+    <col min="3" max="256" customWidth="true" style="1" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert "Committing More missing methods"
This reverts commit 6c042bab6c41e647e49c04a35665ddca893664e2.
</commit_message>
<xml_diff>
--- a/Mendix/input/Mendix_TestPlan.xlsx
+++ b/Mendix/input/Mendix_TestPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Git\MIP\Mendix\input\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="336">
   <si>
     <t>S.NO</t>
   </si>
@@ -1029,25 +1029,12 @@
   </si>
   <si>
     <t>Create Material with Questionnaire only Global - SAP Duplicate Found, Extend Selected</t>
-  </si>
-  <si>
-    <t>Create_Vendor_with_Questionnaire_with_Global_and_Local_JDE</t>
-  </si>
-  <si>
-    <t>SG04</t>
-  </si>
-  <si>
-    <t>1332996</t>
-  </si>
-  <si>
-    <t>14835</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1089,7 +1076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1102,9 +1089,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1445,30 +1429,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:IV13"/>
+  <dimension ref="A1:IV12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="9.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="9.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="75.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="11.109375" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" style="1" width="14.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="13.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="12.44140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="12.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="1" width="10.88671875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="23.109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="1" width="12.44140625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="1" width="12.33203125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="1" width="12.44140625" collapsed="true"/>
-    <col min="17" max="256" customWidth="true" style="1" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="9.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="75.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="14.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.5546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="256" width="9.109375" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2719,7 +2703,7 @@
         <v>335</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>257</v>
+        <v>24</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>333</v>
@@ -2741,41 +2725,6 @@
       </c>
       <c r="K12" s="2" t="s">
         <v>334</v>
-      </c>
-    </row>
-    <row r="13" spans="1:255" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -2799,14 +2748,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="4.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="55.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="24.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="28.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="55.0" collapsed="true"/>
-    <col min="6" max="254" customWidth="true" style="1" width="9.109375" collapsed="true"/>
-    <col min="255" max="255" customWidth="true" style="1" width="4.88671875" collapsed="true"/>
-    <col min="256" max="256" customWidth="true" style="1" width="55.0" collapsed="true"/>
+    <col min="1" max="1" width="4.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="55" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="55" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="254" width="9.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="255" max="255" width="4.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="256" max="256" width="55" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2932,9 +2881,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="22.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="123.109375" collapsed="true"/>
-    <col min="3" max="256" customWidth="true" style="1" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="22.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="123.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="256" width="9.109375" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Committing changes for scripts and also adding few methods
</commit_message>
<xml_diff>
--- a/Mendix/input/Mendix_TestPlan.xlsx
+++ b/Mendix/input/Mendix_TestPlan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="342">
   <si>
     <t>S.NO</t>
   </si>
@@ -1029,6 +1029,24 @@
   </si>
   <si>
     <t>Create Material with Questionnaire only Global - SAP Duplicate Found, Extend Selected</t>
+  </si>
+  <si>
+    <t>Create_Vendor_Happy_flow-with_disable_Local_and_Bank_Request(SAP)</t>
+  </si>
+  <si>
+    <t>Create_Vendor_with_Questionnaire_with_Global_and_Local_JDE</t>
+  </si>
+  <si>
+    <t>SG04</t>
+  </si>
+  <si>
+    <t>1313370</t>
+  </si>
+  <si>
+    <t>14842</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -1429,10 +1447,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:IV12"/>
+  <dimension ref="A1:IV14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2703,7 +2721,7 @@
         <v>335</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>24</v>
+        <v>257</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>333</v>
@@ -2725,6 +2743,76 @@
       </c>
       <c r="K12" s="2" t="s">
         <v>334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:255" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:255" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some changes done in XML File
</commit_message>
<xml_diff>
--- a/Mendix/input/Mendix_TestPlan.xlsx
+++ b/Mendix/input/Mendix_TestPlan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Git\New folder\MIP\Mendix\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Avaniheineken\MIP\Mendix\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA09209-B219-48D7-BD25-5724ADF15CEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="2436"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="2436" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="376">
   <si>
     <t>S.NO</t>
   </si>
@@ -788,6 +789,9 @@
     <t>1</t>
   </si>
   <si>
+    <t>Create_Material</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
@@ -821,33 +825,57 @@
     <t>2</t>
   </si>
   <si>
+    <t>Create_Material_Draft</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
+    <t>Create_Material_Global_Local_NAV</t>
+  </si>
+  <si>
     <t>1377436</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>Create_Material_Global_and_Local_for_JDE</t>
+  </si>
+  <si>
     <t>1416104</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
+    <t>ChangeMaterial_Nav</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
+    <t>ChangeMaterial_Reject_Discard</t>
+  </si>
+  <si>
     <t>1402111</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
+    <t>Create_Vendor_with_Questionnaire_only_Global</t>
+  </si>
+  <si>
     <t>8</t>
   </si>
   <si>
+    <t>Create_Vendor_with_Questionnaire_with_Global_and_Local_and_Bank_JDE</t>
+  </si>
+  <si>
     <t>1416843</t>
   </si>
   <si>
@@ -857,12 +885,63 @@
     <t>BE01</t>
   </si>
   <si>
+    <t>Create with ref Global Only - SAP Direct Copy with Rejections</t>
+  </si>
+  <si>
+    <t>Create Vendor Happy flow - with disable Local and Bank Request(SAP)</t>
+  </si>
+  <si>
+    <t>1420073</t>
+  </si>
+  <si>
+    <t>503159</t>
+  </si>
+  <si>
+    <t>Create Material with Questionnaire only Global - SAP Duplicate Found, Extend Selected</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Create_Vendor_Happy_flow-with_disable_Local_and_Bank_Request(SAP)</t>
+  </si>
+  <si>
+    <t>1421321</t>
+  </si>
+  <si>
+    <t>504364</t>
+  </si>
+  <si>
+    <t>1000114831</t>
+  </si>
+  <si>
     <t>SG04</t>
   </si>
   <si>
+    <t>Create_Vendor_with_Questionnaire_with_Global_and_Local_JDE</t>
+  </si>
+  <si>
+    <t>1313370</t>
+  </si>
+  <si>
+    <t>14842</t>
+  </si>
+  <si>
+    <t>Change _vendor_global _Only</t>
+  </si>
+  <si>
     <t>PA01</t>
   </si>
   <si>
+    <t>Create_Vendor_with_Questionnaire_with_Global_and_Local_NAV</t>
+  </si>
+  <si>
+    <t>DZ01</t>
+  </si>
+  <si>
+    <t>Create_Material_Global_and_Local_for_nav_Duplicate_not_Found</t>
+  </si>
+  <si>
     <t>S.No</t>
   </si>
   <si>
@@ -992,40 +1071,92 @@
     <t>Production | Raw material, ingredient or processing aid</t>
   </si>
   <si>
+    <t>Extend Vendor Global and Local from JDE to  NAV(With Local data adding)</t>
+  </si>
+  <si>
     <t>MZCB</t>
   </si>
   <si>
+    <t>Extend Material Global and Local from SAP to  NAV with Rejections(With Local data adding)</t>
+  </si>
+  <si>
+    <t>1422592</t>
+  </si>
+  <si>
+    <t>47047</t>
+  </si>
+  <si>
     <t>Material Description</t>
   </si>
   <si>
-    <t>14Create Vendor with Questionnaire only Global</t>
-  </si>
-  <si>
-    <t>9Create Material with Questionnaire only Global</t>
-  </si>
-  <si>
-    <t>10Create Material with Questionnaire only Global with Rejections</t>
-  </si>
-  <si>
-    <t>8Create Material Global and Local for nav</t>
-  </si>
-  <si>
-    <t>22Create Vendor with Questionnaire with Global and Local_NAV</t>
-  </si>
-  <si>
-    <t>23Create Vendor with Questionnaire with Global and Local with Rejections_NAV</t>
-  </si>
-  <si>
-    <t>17Create Vendor with Questionnaire with Global and Local_JDE</t>
-  </si>
-  <si>
-    <t>18Create_Vendor_Happy Flow Global and Local with Rejections_JDE</t>
+    <t>Create with ref Global and local - NAV Direct Copy</t>
+  </si>
+  <si>
+    <t>Heineken_Sample_two_one</t>
+  </si>
+  <si>
+    <t>Create Material Global and Local for NAV Duplicate not Found</t>
+  </si>
+  <si>
+    <t>UoM</t>
+  </si>
+  <si>
+    <t>504398</t>
+  </si>
+  <si>
+    <t>1424050</t>
+  </si>
+  <si>
+    <t>416044</t>
+  </si>
+  <si>
+    <t>1424083</t>
+  </si>
+  <si>
+    <t>504412</t>
+  </si>
+  <si>
+    <t>Extend same target system - Extend Global for SAP</t>
+  </si>
+  <si>
+    <t>1424111</t>
+  </si>
+  <si>
+    <t>416057</t>
+  </si>
+  <si>
+    <t>52Happy Flag for deletion(Not Shared with Multi OpCos) - JDE_Material</t>
+  </si>
+  <si>
+    <t>416495</t>
+  </si>
+  <si>
+    <t>1425554</t>
+  </si>
+  <si>
+    <t>46Extend_same_target system - Extend_Global_and_Local_for_Non_SAP JDE</t>
+  </si>
+  <si>
+    <t>416496</t>
+  </si>
+  <si>
+    <t>1425569</t>
+  </si>
+  <si>
+    <t>416501</t>
+  </si>
+  <si>
+    <t>51.Happy Flag For Deletion(Not Shared With Multiple Opcos)_SAP</t>
+  </si>
+  <si>
+    <t>1425585</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1431,30 +1562,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:IV24"/>
+  <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="75.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="14.109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13" style="2" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.88671875" style="2" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23" style="2" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.33203125" style="2" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="17" max="256" width="9.109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="9.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="75.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="9.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="11.109375" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" style="2" width="14.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="2" width="13.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="2" width="12.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="2" width="10.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="2" width="23.109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="2" width="23.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="2" width="12.33203125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
+    <col min="17" max="256" customWidth="true" style="2" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1507,7 +1640,7 @@
         <v>15</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>324</v>
+        <v>354</v>
       </c>
       <c r="R1" s="7" t="s">
         <v>16</v>
@@ -2229,49 +2362,49 @@
         <v>254</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>325</v>
+        <v>55</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>255</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>23</v>
+        <v>256</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -2515,52 +2648,52 @@
     </row>
     <row r="3" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>277</v>
+        <v>55</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>326</v>
+        <v>267</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -2804,52 +2937,52 @@
     </row>
     <row r="4" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>327</v>
+        <v>128</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>269</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
@@ -3093,52 +3226,52 @@
     </row>
     <row r="5" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>323</v>
+        <v>272</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>328</v>
+        <v>273</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
@@ -3382,52 +3515,52 @@
     </row>
     <row r="6" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>267</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
@@ -3671,170 +3804,196 @@
     </row>
     <row r="7" spans="1:255" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>272</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M7" s="4">
         <v>30007783</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:255" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>278</v>
+        <v>55</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>331</v>
+        <v>281</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M8" s="4">
         <v>30007783</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:255" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>332</v>
+        <v>283</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M9" s="4">
         <v>30007783</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>359</v>
+      </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+      <c r="N10" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>265</v>
+      </c>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
@@ -4077,21 +4236,47 @@
       <c r="IU10" s="4"/>
     </row>
     <row r="11" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>290</v>
+      </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
+      <c r="N11" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>265</v>
+      </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
@@ -4334,21 +4519,49 @@
       <c r="IU11" s="4"/>
     </row>
     <row r="12" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="4">
+        <v>27787</v>
+      </c>
+      <c r="L12" s="4">
+        <v>30007258</v>
+      </c>
       <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
+      <c r="N12" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>265</v>
+      </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
@@ -4591,21 +4804,49 @@
       <c r="IU12" s="4"/>
     </row>
     <row r="13" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>296</v>
+      </c>
       <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
+      <c r="N13" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>265</v>
+      </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
@@ -4848,21 +5089,47 @@
       <c r="IU13" s="4"/>
     </row>
     <row r="14" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>300</v>
+      </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
+      <c r="N14" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>265</v>
+      </c>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
@@ -5105,21 +5372,47 @@
       <c r="IU14" s="4"/>
     </row>
     <row r="15" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="A15" s="5">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>300</v>
+      </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+      <c r="N15" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>265</v>
+      </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
@@ -5362,21 +5655,47 @@
       <c r="IU15" s="4"/>
     </row>
     <row r="16" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="A16" s="5">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>363</v>
+      </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
+      <c r="N16" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>265</v>
+      </c>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
@@ -5619,21 +5938,51 @@
       <c r="IU16" s="4"/>
     </row>
     <row r="17" spans="1:255" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
+      <c r="A17" s="5">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>265</v>
+      </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
@@ -5876,17 +6225,39 @@
       <c r="IU17" s="9"/>
     </row>
     <row r="18" spans="1:255" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
+      <c r="A18" s="8">
+        <v>16</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E18" s="7">
+        <v>1421407</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="7">
+        <v>14841</v>
+      </c>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
@@ -6133,17 +6504,39 @@
       <c r="IU18" s="7"/>
     </row>
     <row r="19" spans="1:255" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="10"/>
+      <c r="A19" s="8">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>353</v>
+      </c>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
@@ -6390,23 +6783,57 @@
       <c r="IU19" s="7"/>
     </row>
     <row r="20" spans="1:255" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="7"/>
+      <c r="A20" s="8">
+        <v>18</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1421407</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="7">
+        <v>34506</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>356</v>
+      </c>
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
       <c r="T20" s="7"/>
@@ -6647,17 +7074,39 @@
       <c r="IU20" s="7"/>
     </row>
     <row r="21" spans="1:255" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
+      <c r="A21" s="8">
+        <v>19</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>361</v>
+      </c>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
@@ -6904,17 +7353,39 @@
       <c r="IU21" s="7"/>
     </row>
     <row r="22" spans="1:255" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
+      <c r="A22" s="8">
+        <v>20</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E22" s="7">
+        <v>1423997</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>359</v>
+      </c>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
@@ -7161,20 +7632,176 @@
       <c r="IU22" s="7"/>
     </row>
     <row r="23" spans="1:255" x14ac:dyDescent="0.25">
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="24" spans="1:255" x14ac:dyDescent="0.25">
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="25" spans="1:255" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="26" spans="1:255" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="27" spans="1:255" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>373</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7187,7 +7814,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:IV6"/>
   <sheetViews>
@@ -7197,31 +7824,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="55" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.6640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="55" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="254" width="9.109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="255" max="255" width="4.88671875" style="2" customWidth="1" collapsed="1"/>
-    <col min="256" max="256" width="55" style="2" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="4.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="55.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="24.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="28.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="55.0" collapsed="true"/>
+    <col min="6" max="254" customWidth="true" style="2" width="9.109375" collapsed="true"/>
+    <col min="255" max="255" customWidth="true" style="2" width="4.88671875" collapsed="true"/>
+    <col min="256" max="256" customWidth="true" style="2" width="55.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>281</v>
+        <v>307</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>282</v>
+        <v>308</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>283</v>
+        <v>309</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>284</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -7229,84 +7856,84 @@
         <v>254</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>285</v>
+        <v>311</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>286</v>
+        <v>312</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>287</v>
+        <v>313</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>285</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>288</v>
+        <v>314</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>286</v>
+        <v>312</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>289</v>
+        <v>315</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>288</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>290</v>
+        <v>316</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>286</v>
+        <v>312</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>289</v>
+        <v>315</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>290</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>286</v>
+        <v>312</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>289</v>
+        <v>315</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>291</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>292</v>
+        <v>318</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>286</v>
+        <v>312</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>289</v>
+        <v>315</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>292</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -7320,7 +7947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:IV21"/>
   <sheetViews>
@@ -7330,38 +7957,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="123.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="256" width="9.109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="22.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="123.109375" collapsed="true"/>
+    <col min="3" max="256" customWidth="true" style="2" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>293</v>
+        <v>319</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>294</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>295</v>
+        <v>321</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>296</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>297</v>
+        <v>323</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>298</v>
+        <v>324</v>
       </c>
       <c r="B4" s="1">
         <v>30</v>
@@ -7369,7 +7996,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>299</v>
+        <v>325</v>
       </c>
       <c r="B5" s="1">
         <v>30</v>
@@ -7377,7 +8004,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>300</v>
+        <v>326</v>
       </c>
       <c r="B6" s="1">
         <v>30</v>
@@ -7385,7 +8012,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>301</v>
+        <v>327</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -7393,7 +8020,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>302</v>
+        <v>328</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -7401,7 +8028,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>303</v>
+        <v>329</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
@@ -7409,7 +8036,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>304</v>
+        <v>330</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
@@ -7417,7 +8044,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>305</v>
+        <v>331</v>
       </c>
       <c r="B11" s="1">
         <v>5</v>
@@ -7425,7 +8052,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>306</v>
+        <v>332</v>
       </c>
       <c r="B12" s="1">
         <v>6</v>
@@ -7433,39 +8060,39 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>307</v>
+        <v>333</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>308</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>309</v>
+        <v>335</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>310</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>311</v>
+        <v>337</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>312</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>313</v>
+        <v>339</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>314</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>315</v>
+        <v>341</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>237</v>
@@ -7473,23 +8100,23 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>316</v>
+        <v>342</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>317</v>
+        <v>343</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>318</v>
+        <v>344</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>319</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>320</v>
+        <v>346</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>55</v>
@@ -7497,10 +8124,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>321</v>
+        <v>347</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>322</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>